<commit_message>
Zastosowanie wzorca projektowego MCV
</commit_message>
<xml_diff>
--- a/MyBarcodeFile.xlsx
+++ b/MyBarcodeFile.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Teresa</t>
   </si>
@@ -43,7 +43,10 @@
     <t>zrzóśżó</t>
   </si>
   <si>
-    <t>asd</t>
+    <t>Julitka</t>
+  </si>
+  <si>
+    <t>Doma}ska</t>
   </si>
 </sst>
 </file>
@@ -379,7 +382,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -392,10 +395,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C1" s="1">
+        <v>300621357439</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>

<commit_message>
Zastosowanie wzorca projektowego MCV Zmiana pola static int iteration(globalna) na pole int iteration wewnątrz kodu
</commit_message>
<xml_diff>
--- a/MyBarcodeFile.xlsx
+++ b/MyBarcodeFile.xlsx
@@ -46,7 +46,7 @@
     <t>Julitka</t>
   </si>
   <si>
-    <t>Doma}ska</t>
+    <t>Domańska</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -392,10 +392,10 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
       </c>
       <c r="C1" s="1">
         <v>300621357439</v>
@@ -403,10 +403,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
       <c r="C2" s="1">
         <v>300621332788</v>
@@ -414,10 +414,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
       <c r="C3" s="1">
         <v>300621349319</v>
@@ -425,10 +425,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>300621357439</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
       </c>
       <c r="C5" s="1">
         <v>300621360914</v>
@@ -447,10 +447,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
         <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>300621360914</v>

</xml_diff>